<commit_message>
Add menu for spring 2024 * wef 16/01/2024
</commit_message>
<xml_diff>
--- a/excel_menu/yuktahar_old.xlsx
+++ b/excel_menu/yuktahar_old.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vjspranav/Projects/making_table/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vjspranav/Projects/IIITMessMenu/excel_menu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774224BC-2664-514C-B9FD-824E237E80B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD845CB9-4B32-B448-B420-EA0027BBBD1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="121">
   <si>
     <t>ITEM1</t>
   </si>
@@ -49,7 +49,7 @@
     <t>Veg Poha</t>
   </si>
   <si>
-    <t>Jowari roti</t>
+    <t>Whole wheat bread</t>
   </si>
   <si>
     <t>ITEM2</t>
@@ -61,23 +61,23 @@
     <t>Raagi + Butter Milk</t>
   </si>
   <si>
-    <t>Plain Daliya</t>
+    <t>Chilla + Mint Chutney</t>
   </si>
   <si>
     <t>Raagi+Butter Milk</t>
   </si>
   <si>
-    <t>Raajgira</t>
+    <t>Raajgira + Oats</t>
   </si>
   <si>
     <t>Plain daliya</t>
   </si>
   <si>
-    <t>Hummus+ Salad</t>
-  </si>
-  <si>
-    <t>ACCOMPANIME
-NTS</t>
+    <t>Hummus+ Salad + Upma</t>
+  </si>
+  <si>
+    <t>ACCOMPANI
+MENTS</t>
   </si>
   <si>
     <t>Sambhar + Cocount
@@ -87,14 +87,16 @@
     <t>Groundnut Chutney</t>
   </si>
   <si>
-    <t>Putana chutney+Sambar</t>
+    <t>Putana
+chutney+Sambar</t>
   </si>
   <si>
     <t>Putana Chutney</t>
   </si>
   <si>
     <t>Sambhar + Tomato
-chutney/Coconut chutney</t>
+chutney/Coconut
+chutney</t>
   </si>
   <si>
     <t>Coconut chutney</t>
@@ -124,8 +126,7 @@
     <t>Curd Rice</t>
   </si>
   <si>
-    <t>Foxtail (Korralu) Millet
-Pulao</t>
+    <t>Foxtail (Korralu) Millet Pulao</t>
   </si>
   <si>
     <t>Roti</t>
@@ -134,7 +135,7 @@
     <t>Live Roti</t>
   </si>
   <si>
-    <t>Live Bhajra Roti</t>
+    <t>Live Jawari Roti</t>
   </si>
   <si>
     <t>Live roti</t>
@@ -150,6 +151,9 @@
     <t>Masoor Dal</t>
   </si>
   <si>
+    <t>Dal Fry</t>
+  </si>
+  <si>
     <t>Gongura dal</t>
   </si>
   <si>
@@ -159,6 +163,9 @@
     <t>Tomato dal</t>
   </si>
   <si>
+    <t>Pumpkin Curry / Dal</t>
+  </si>
+  <si>
     <t>Vegetable</t>
   </si>
   <si>
@@ -171,16 +178,13 @@
     <t>Aloo Methi</t>
   </si>
   <si>
-    <t>Soyabean</t>
-  </si>
-  <si>
     <t>Beetroot Poriyal</t>
   </si>
   <si>
     <t>Beans &amp; Carrot Poriyal</t>
   </si>
   <si>
-    <t>Pumpkin Curry / Dal</t>
+    <t>Black Chana Curry</t>
   </si>
   <si>
     <t>Extra</t>
@@ -189,7 +193,7 @@
     <t>Sambar</t>
   </si>
   <si>
-    <t>Palak Paneer</t>
+    <t>Matar Paneer</t>
   </si>
   <si>
     <t>Mah chhole</t>
@@ -198,109 +202,100 @@
     <t>Dahi Kadhi</t>
   </si>
   <si>
-    <t>Black Chana Curry</t>
+    <t>Masala Papad</t>
   </si>
   <si>
     <t>Chutney</t>
   </si>
   <si>
-    <t>Gongura chutney</t>
+    <t>Ridge gourd chutney</t>
   </si>
   <si>
     <t>Dosakai chutney</t>
   </si>
   <si>
-    <t>tomato chutney</t>
-  </si>
-  <si>
-    <t>Ridge gourd chutney</t>
+    <t>Gongura Chutney</t>
   </si>
   <si>
     <t>kandi pacchadi</t>
   </si>
   <si>
-    <t>Pudina &amp; Tomato Chutney</t>
+    <t>Karela Chutney</t>
   </si>
   <si>
     <t>Sweet</t>
   </si>
   <si>
-    <t>Flaxseed / Peanut Laddu</t>
-  </si>
-  <si>
-    <t>Ravva Laddu</t>
-  </si>
-  <si>
-    <t>Daliya Sweet / Fruit
-Custard</t>
+    <t>Rawa Laddu</t>
+  </si>
+  <si>
+    <t>Flaxseed+Peanut
+Laddu</t>
+  </si>
+  <si>
+    <t>Daliya Sweet / Fruit Custard</t>
   </si>
   <si>
     <t>Rice + Buttermilk + Kichidi + Salad</t>
   </si>
   <si>
-    <t>Uttappam + Coriander
-chutney</t>
-  </si>
-  <si>
-    <t>multi flour Sarvapindi with
-imli chutney</t>
-  </si>
-  <si>
-    <t>Seasoned Salad of boiled
-Chhole, Beans and
-Peanuts + Green Dhaniya
+    <t>Steamed Corn and Badam
+Milk</t>
+  </si>
+  <si>
+    <t>Uttappam+Coriander
 Chutney</t>
   </si>
   <si>
+    <t>Masala Oats +
+Chutney</t>
+  </si>
+  <si>
     <t>Ragi Dosa + Chutney</t>
   </si>
   <si>
-    <t>Masala Oats + Chutney+ Curd</t>
-  </si>
-  <si>
-    <t>Steamed Corn / Chilla + Badam
+    <t>Seasoned Salad of
+boiled Chhole, Beans
+and Peanuts + Green</t>
+  </si>
+  <si>
+    <t>Louki ka Chilla + Badam
 Thandai</t>
   </si>
   <si>
-    <t>Sweet Potato / Peanut
-Chat + Lassi</t>
+    <t>Sweet Potato / Peanut Chat +
+Lassi</t>
   </si>
   <si>
     <t>RICE</t>
   </si>
   <si>
-    <t>Mint Rice</t>
-  </si>
-  <si>
-    <t>Coconut / Jeera Rice</t>
+    <t>Tomato Rice</t>
+  </si>
+  <si>
+    <t>Jeera Rice</t>
+  </si>
+  <si>
+    <t>Coconut Rice</t>
   </si>
   <si>
     <t>Ragi sangati</t>
   </si>
   <si>
-    <t>Masala Khichidi-Dry</t>
-  </si>
-  <si>
-    <t>Tomato Rice</t>
-  </si>
-  <si>
-    <t>Methi Roti</t>
-  </si>
-  <si>
-    <t>Live Palak Roti</t>
-  </si>
-  <si>
-    <t>Beetroot Roti</t>
-  </si>
-  <si>
-    <t>Mango dal</t>
+    <t>Masala kichdi</t>
+  </si>
+  <si>
+    <t>Corn &amp; Peas Pulao</t>
+  </si>
+  <si>
+    <t>Toor dal</t>
   </si>
   <si>
     <t>Mix dal / Panchrang Dal [with
 and without onion]</t>
   </si>
   <si>
-    <t>leafy moong dal with tadka</t>
+    <t>Moong dal tadka</t>
   </si>
   <si>
     <t>Daal Makhni</t>
@@ -309,7 +304,7 @@
     <t>Lobiya</t>
   </si>
   <si>
-    <t>Thotakura dal</t>
+    <t>Black Urad Dal</t>
   </si>
   <si>
     <t>Black Masoor Dal</t>
@@ -318,16 +313,16 @@
     <t>Baingan Bartha</t>
   </si>
   <si>
-    <t>Bhindi</t>
+    <t>Cabbage Porial</t>
   </si>
   <si>
     <t>Lauki</t>
   </si>
   <si>
-    <t>Gawar Phali</t>
-  </si>
-  <si>
-    <t>Turai-Chana dal Sabzi</t>
+    <t>Flat Beans</t>
+  </si>
+  <si>
+    <t>Thurai</t>
   </si>
   <si>
     <t>Dry mix veg</t>
@@ -339,7 +334,7 @@
     <t>Rasam</t>
   </si>
   <si>
-    <t>Pachipulusu</t>
+    <t>Sambar/ Gatte ka Sabji</t>
   </si>
   <si>
     <t>Donda Chutney</t>
@@ -351,6 +346,10 @@
     <t>Palli Podi</t>
   </si>
   <si>
+    <t>Pudina + Tomato
+chutney</t>
+  </si>
+  <si>
     <t>coconut podi</t>
   </si>
   <si>
@@ -360,12 +359,18 @@
     <t>Semiya Payasam</t>
   </si>
   <si>
-    <t>Suji / Lauki Halwa</t>
+    <t>Gazar halwa</t>
   </si>
   <si>
     <t>Item</t>
   </si>
   <si>
+    <t>Compulsory</t>
+  </si>
+  <si>
+    <t>Meal</t>
+  </si>
+  <si>
     <t>Items</t>
   </si>
   <si>
@@ -375,37 +380,31 @@
     <t>Tuesday</t>
   </si>
   <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Breakfast</t>
+  </si>
+  <si>
+    <t>Lunch</t>
+  </si>
+  <si>
+    <t>Dinner</t>
+  </si>
+  <si>
+    <t>Snacks</t>
+  </si>
+  <si>
     <t>Wednesday</t>
-  </si>
-  <si>
-    <t>Thursday</t>
-  </si>
-  <si>
-    <t>Friday</t>
-  </si>
-  <si>
-    <t>Saturday</t>
-  </si>
-  <si>
-    <t>Sunday</t>
-  </si>
-  <si>
-    <t>Breakfast</t>
-  </si>
-  <si>
-    <t>Lunch</t>
-  </si>
-  <si>
-    <t>Snack</t>
-  </si>
-  <si>
-    <t>Dinner</t>
-  </si>
-  <si>
-    <t>Meal</t>
-  </si>
-  <si>
-    <t>Compulsory</t>
   </si>
 </sst>
 </file>
@@ -423,13 +422,13 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="8.5"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="7.5"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -467,9 +466,18 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="4">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -499,134 +507,73 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -942,141 +889,141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="25.83203125" customWidth="1"/>
-    <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" customWidth="1"/>
-    <col min="7" max="7" width="27" customWidth="1"/>
-    <col min="8" max="8" width="27.33203125" customWidth="1"/>
-    <col min="9" max="9" width="21" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" customWidth="1"/>
+    <col min="4" max="4" width="24.5" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" customWidth="1"/>
+    <col min="7" max="7" width="19.5" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" customWidth="1"/>
+    <col min="9" max="9" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="6" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3"/>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3"/>
       <c r="B4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="8" t="s">
         <v>22</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3"/>
       <c r="B5" s="19" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="C5" t="s">
         <v>24</v>
@@ -1093,14 +1040,14 @@
       <c r="G5" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="H5" s="24" t="s">
         <v>24</v>
       </c>
       <c r="I5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>117</v>
       </c>
@@ -1129,7 +1076,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2"/>
       <c r="B7" s="10" t="s">
         <v>32</v>
@@ -1156,7 +1103,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2"/>
       <c r="B8" s="10" t="s">
         <v>36</v>
@@ -1167,82 +1114,82 @@
       <c r="D8" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="13"/>
+      <c r="E8" s="13" t="s">
+        <v>39</v>
+      </c>
       <c r="F8" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="I8" s="14"/>
-    </row>
-    <row r="9" spans="1:9" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>42</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>46</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="F9" s="14"/>
       <c r="G9" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2"/>
       <c r="B10" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="13"/>
+        <v>51</v>
+      </c>
+      <c r="C10" s="14"/>
       <c r="D10" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="12" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H10" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I10" s="15"/>
+    </row>
+    <row r="11" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2"/>
       <c r="B11" s="10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="11" t="s">
         <v>59</v>
       </c>
+      <c r="E11" s="14"/>
       <c r="F11" s="11" t="s">
         <v>60</v>
       </c>
@@ -1252,31 +1199,33 @@
       <c r="H11" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="I11" s="14"/>
-    </row>
-    <row r="12" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I11" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2"/>
       <c r="B12" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
+      <c r="C12" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="14"/>
       <c r="E12" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="H12" s="13"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
       <c r="I12" s="12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2"/>
       <c r="B13" s="19" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="C13" t="s">
         <v>67</v>
@@ -1293,19 +1242,19 @@
       <c r="G13" t="s">
         <v>67</v>
       </c>
-      <c r="H13" s="26" t="s">
+      <c r="H13" s="24" t="s">
         <v>67</v>
       </c>
       <c r="I13" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>107</v>
+    <row r="14" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>106</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>68</v>
@@ -1329,40 +1278,42 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>75</v>
       </c>
       <c r="C15" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="F15" s="20"/>
       <c r="G15" s="19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H15" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="I15" s="21" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I15" s="20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="18" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="D16" s="19" t="s">
         <v>33</v>
@@ -1371,139 +1322,139 @@
         <v>33</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="G16" s="19" t="s">
         <v>33</v>
       </c>
       <c r="H16" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="I16" s="21" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I16" s="20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
       <c r="B17" s="18" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="F17" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="G17" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="F17" s="19" t="s">
+      <c r="H17" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="G17" s="19" t="s">
+      <c r="I17" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="H17" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="I17" s="21" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="18" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1"/>
       <c r="B18" s="18" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C18" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="F18" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="G18" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="F18" s="19" t="s">
+      <c r="H18" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="G18" s="19" t="s">
+      <c r="I18" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="H18" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="I18" s="21" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="19" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1"/>
       <c r="B19" s="18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="H19" s="20"/>
-      <c r="I19" s="23" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>96</v>
+      </c>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="22"/>
+    </row>
+    <row r="20" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1"/>
       <c r="B20" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C20" s="19" t="s">
         <v>23</v>
       </c>
       <c r="D20" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F20" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="G20" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="F20" s="19" t="s">
+      <c r="H20" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="I20" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="G20" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="H20" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="I20" s="24"/>
-    </row>
-    <row r="21" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="21" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
       <c r="B21" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="20"/>
+      <c r="C21" s="21"/>
       <c r="D21" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="E21" s="21"/>
+      <c r="F21" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="E21" s="20"/>
-      <c r="F21" s="19" t="s">
+      <c r="G21" s="21"/>
+      <c r="H21" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="G21" s="20"/>
-      <c r="H21" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="I21" s="24"/>
-    </row>
-    <row r="22" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I21" s="22"/>
+    </row>
+    <row r="22" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1"/>
       <c r="B22" s="19" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="C22" t="s">
         <v>67</v>
@@ -1520,26 +1471,16 @@
       <c r="G22" t="s">
         <v>67</v>
       </c>
-      <c r="H22" s="26" t="s">
+      <c r="H22" s="24" t="s">
         <v>67</v>
       </c>
       <c r="I22" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="E27" s="27"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="29"/>
-    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A15:A22"/>
-    <mergeCell ref="E27:K27"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A13"/>
   </mergeCells>

</xml_diff>